<commit_message>
started to add in Gauge tests
</commit_message>
<xml_diff>
--- a/Experiments/Standard Data and API Experiments.xlsx
+++ b/Experiments/Standard Data and API Experiments.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Fly Fishing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Fly Fishing\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21096" windowHeight="7164"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21096" windowHeight="7164" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="States" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="124">
   <si>
     <t>State</t>
   </si>
@@ -330,6 +332,72 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Variety</t>
+  </si>
+  <si>
+    <t>Trout</t>
+  </si>
+  <si>
+    <t>Rainbow</t>
+  </si>
+  <si>
+    <t>Cutthroat</t>
+  </si>
+  <si>
+    <t>Brook</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Sea</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>Spake</t>
+  </si>
+  <si>
+    <t>Bull</t>
+  </si>
+  <si>
+    <t>Golden</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Dolly Vardon</t>
+  </si>
+  <si>
+    <t>Bass</t>
+  </si>
+  <si>
+    <t>Smallmouth</t>
+  </si>
+  <si>
+    <t>Largemouth</t>
+  </si>
+  <si>
+    <t>Peacock</t>
+  </si>
+  <si>
+    <t>Striped</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Yellow</t>
   </si>
 </sst>
 </file>
@@ -692,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
@@ -885,7 +953,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -893,7 +961,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -933,7 +1001,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -941,7 +1009,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -949,7 +1017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -989,7 +1057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -1005,7 +1073,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -1013,7 +1081,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -1029,7 +1097,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -1037,7 +1105,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -1077,7 +1145,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -1085,7 +1153,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -1093,7 +1161,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -1165,4 +1233,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId51"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>